<commit_message>
add temp one match, two match
add temp one match, two match
prepare for two match compute
</commit_message>
<xml_diff>
--- a/net_helper/data/DataTable.xlsx
+++ b/net_helper/data/DataTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Match" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="92">
   <si>
     <t>timespan</t>
   </si>
@@ -256,6 +256,47 @@
   </si>
   <si>
     <t>half_l_l</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>point_w……</t>
+  </si>
+  <si>
+    <t>point_l……</t>
+  </si>
+  <si>
+    <t>ww,dw,lw</t>
+  </si>
+  <si>
+    <t>wd,dd,ld</t>
+  </si>
+  <si>
+    <t>wl,dl,ll</t>
+  </si>
+  <si>
+    <t>point_d……</t>
+  </si>
+  <si>
+    <t>spread_d=(point_w_1_0+point _w_2_1+
+                      point_w_3_2+point_w_other)</t>
+  </si>
+  <si>
+    <t>spread_w =wdl-
+                      (point_w_1_0,point _w_2_1,
+                       point_w_3_2,point_w_other)</t>
+  </si>
+  <si>
+    <t>spread_l=wdl_l +(point_d_0_0+  point_d_1_1….)
+or
+spread_l=wdl_l+wdl_d</t>
   </si>
 </sst>
 </file>
@@ -753,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1242,12 +1283,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60">
+      <c r="A3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>